<commit_message>
Menambahkan folder pertemuan 3,4, dan 5
</commit_message>
<xml_diff>
--- a/Dokumentasi/html.xlsx
+++ b/Dokumentasi/html.xlsx
@@ -5,20 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myFolder\App\Dokumentasi\belajarweb-html\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myFolder\App\app_tutorial\app_KT\belajarweb-html\Dokumentasi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F8F714-371F-4AF9-B70B-8FB44D50925F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B1106F-C625-4210-9430-559D1D8DC80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11560" yWindow="1900" windowWidth="7680" windowHeight="7270" xr2:uid="{BE55DF2D-4F83-451E-8655-75B2D0DC4CEB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BE55DF2D-4F83-451E-8655-75B2D0DC4CEB}"/>
   </bookViews>
   <sheets>
-    <sheet name="6" sheetId="6" r:id="rId1"/>
-    <sheet name="5" sheetId="5" r:id="rId2"/>
-    <sheet name="4" sheetId="4" r:id="rId3"/>
-    <sheet name="3" sheetId="3" r:id="rId4"/>
-    <sheet name="2" sheetId="2" r:id="rId5"/>
-    <sheet name="1" sheetId="1" r:id="rId6"/>
+    <sheet name="8" sheetId="8" r:id="rId1"/>
+    <sheet name="7" sheetId="6" r:id="rId2"/>
+    <sheet name="6" sheetId="7" r:id="rId3"/>
+    <sheet name="5" sheetId="5" r:id="rId4"/>
+    <sheet name="4" sheetId="4" r:id="rId5"/>
+    <sheet name="3" sheetId="3" r:id="rId6"/>
+    <sheet name="2" sheetId="2" r:id="rId7"/>
+    <sheet name="1" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>T</t>
   </si>
@@ -102,13 +104,25 @@
   </si>
   <si>
     <t>Underline, superscript, subscript</t>
+  </si>
+  <si>
+    <t>Storng, emphasis, blockqute, quote</t>
+  </si>
+  <si>
+    <t>Line Break</t>
+  </si>
+  <si>
+    <t>Horizontal Rules</t>
+  </si>
+  <si>
+    <t>Tag Extra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +138,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -151,10 +173,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -173,6 +196,493 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>343168</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114467</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{510D0AB0-EF9C-CDF2-B96C-C455A8AD6E91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="368300"/>
+          <a:ext cx="5219968" cy="3245017"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>553552</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54EDB909-FFEB-C76C-D3E8-5841552CCC96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5492750" y="463550"/>
+          <a:ext cx="6643202" cy="3108960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:shade val="85000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="88900" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="55000" dist="18000" dir="5400000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="twoPt" dir="t">
+            <a:rot lat="0" lon="0" rev="7200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="25400" h="19050"/>
+          <a:contourClr>
+            <a:srgbClr val="FFFFFF"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>539966</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>70126</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FED4716-4A1F-E0CD-DB5F-F849BF41C25F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="266700"/>
+          <a:ext cx="4197566" cy="5378726"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>482872</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>76293</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7567CA2-6A0F-1CBF-B24B-447EC0329284}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4343400" y="336550"/>
+          <a:ext cx="5283472" cy="1816193"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:shade val="85000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="88900" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="55000" dist="18000" dir="5400000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="twoPt" dir="t">
+            <a:rot lat="0" lon="0" rev="7200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="25400" h="19050"/>
+          <a:contourClr>
+            <a:srgbClr val="FFFFFF"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57341</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>89017</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A193B0E7-A8B6-A8FB-E61F-8C4019039FAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="260350"/>
+          <a:ext cx="3714941" cy="2273417"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>597087</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>88999</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80DA0F09-855A-8BBF-C3A7-51138B31D21C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3048000"/>
+          <a:ext cx="3645087" cy="1930499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57263</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>71</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{453B300D-195C-C608-6599-DB71D23A013B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3956050" y="3130550"/>
+          <a:ext cx="2197213" cy="1390721"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:shade val="85000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="88900" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="55000" dist="18000" dir="5400000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="twoPt" dir="t">
+            <a:rot lat="0" lon="0" rev="7200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="25400" h="19050"/>
+          <a:contourClr>
+            <a:srgbClr val="FFFFFF"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>520810</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>133400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D8DE458-6220-C1D3-2BB8-66F137EE797D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3873500" y="311150"/>
+          <a:ext cx="2133710" cy="977950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:shade val="85000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="88900" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="55000" dist="18000" dir="5400000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="twoPt" dir="t">
+            <a:rot lat="0" lon="0" rev="7200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="25400" h="19050"/>
+          <a:contourClr>
+            <a:srgbClr val="FFFFFF"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -265,7 +775,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -684,32 +1194,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E112F0-2E17-4E9A-8639-5F4D24A5E810}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A93DA0E-B778-4525-B76C-20E473A2F392}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22055E12-B76B-4F4B-A3D5-DF3C18DCD5FD}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>23</v>
+    <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E112F0-2E17-4E9A-8639-5F4D24A5E810}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B05D21F-9E4B-4394-9209-F70724D368DC}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -718,51 +1263,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B153817C-D04A-423F-9EA3-07E755361F3C}">
-  <dimension ref="A1:B6"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22055E12-B76B-4F4B-A3D5-DF3C18DCD5FD}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
+    <row r="1" spans="1:1" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -771,12 +1282,63 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B153817C-D04A-423F-9EA3-07E755361F3C}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1A47AF-1727-4E7B-812A-11B99171AFE2}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -791,7 +1353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9314D0C6-3FBB-470F-ADCC-828AFCE2130B}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -830,7 +1392,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E7786A-4E8F-4BCC-BF91-0AB432E29399}">
   <dimension ref="A1:B6"/>
   <sheetViews>

</xml_diff>